<commit_message>
pres and time investigation
</commit_message>
<xml_diff>
--- a/times2test.xlsx
+++ b/times2test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\install\SemLink\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian Leprevost\Documents\SemLink\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEDB56D-F21A-49F1-AA7B-E120E1DCA7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB116AC-CC9A-457B-B9DF-DD1CC76B5584}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{7DCE6840-0CB1-499F-AB4F-E0D786E07834}"/>
+    <workbookView minimized="1" xWindow="-114" yWindow="-114" windowWidth="23254" windowHeight="13174" activeTab="3" xr2:uid="{7DCE6840-0CB1-499F-AB4F-E0D786E07834}"/>
   </bookViews>
   <sheets>
     <sheet name="precond1" sheetId="1" r:id="rId1"/>
@@ -19,19 +19,10 @@
     <sheet name="inference" sheetId="4" r:id="rId4"/>
     <sheet name="inferenceadjusted" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -144,7 +135,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -446,9 +437,9 @@
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1680</v>
       </c>
@@ -459,7 +450,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1680</v>
       </c>
@@ -470,7 +461,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1680</v>
       </c>
@@ -481,7 +472,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>4760</v>
       </c>
@@ -492,7 +483,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1680</v>
       </c>
@@ -503,7 +494,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3360</v>
       </c>
@@ -514,7 +505,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1960</v>
       </c>
@@ -525,7 +516,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1960</v>
       </c>
@@ -536,7 +527,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1400</v>
       </c>
@@ -547,7 +538,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2240</v>
       </c>
@@ -558,7 +549,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>3080</v>
       </c>
@@ -569,7 +560,7 @@
         <v>2240</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>3080</v>
       </c>
@@ -580,7 +571,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>3640</v>
       </c>
@@ -591,7 +582,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1960</v>
       </c>
@@ -602,7 +593,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2520</v>
       </c>
@@ -613,7 +604,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1680</v>
       </c>
@@ -624,7 +615,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2520</v>
       </c>
@@ -635,7 +626,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>3640</v>
       </c>
@@ -646,7 +637,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>1960</v>
       </c>
@@ -657,7 +648,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>1680</v>
       </c>
@@ -668,7 +659,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>1680</v>
       </c>
@@ -679,7 +670,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>1680</v>
       </c>
@@ -690,7 +681,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>4760</v>
       </c>
@@ -701,7 +692,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1680</v>
       </c>
@@ -712,7 +703,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>3360</v>
       </c>
@@ -723,7 +714,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>1960</v>
       </c>
@@ -734,7 +725,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>1960</v>
       </c>
@@ -745,7 +736,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>1400</v>
       </c>
@@ -756,7 +747,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>2240</v>
       </c>
@@ -767,7 +758,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>3080</v>
       </c>
@@ -778,7 +769,7 @@
         <v>2240</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>3080</v>
       </c>
@@ -789,7 +780,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>3640</v>
       </c>
@@ -800,7 +791,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>1960</v>
       </c>
@@ -811,7 +802,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>2520</v>
       </c>
@@ -822,7 +813,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>1680</v>
       </c>
@@ -833,7 +824,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>2520</v>
       </c>
@@ -844,7 +835,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>3640</v>
       </c>
@@ -855,7 +846,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>1960</v>
       </c>
@@ -866,7 +857,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>2240</v>
       </c>
@@ -877,7 +868,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>17000</v>
       </c>
@@ -888,7 +879,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -896,36 +887,36 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
       <c r="B42">
-        <f>SUM(B1:B41)</f>
+        <f t="shared" ref="B42:G42" si="0">SUM(B1:B41)</f>
         <v>113200</v>
       </c>
       <c r="C42">
-        <f>SUM(C1:C41)</f>
+        <f t="shared" si="0"/>
         <v>105200</v>
       </c>
       <c r="D42">
-        <f>SUM(D1:D41)</f>
+        <f t="shared" si="0"/>
         <v>102400</v>
       </c>
       <c r="E42">
-        <f>SUM(E1:E41)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F42">
-        <f>SUM(F1:F41)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G42">
-        <f>SUM(G1:G41)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -938,23 +929,23 @@
         <v>105.2</v>
       </c>
       <c r="D43">
-        <f t="shared" ref="D43:G43" si="0">D42/1000</f>
+        <f t="shared" ref="D43:G43" si="1">D42/1000</f>
         <v>102.4</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -967,23 +958,23 @@
         <v>102.2</v>
       </c>
       <c r="D44">
-        <f t="shared" ref="D44:G44" si="1">D43-3</f>
+        <f t="shared" ref="D44:G44" si="2">D43-3</f>
         <v>99.4</v>
       </c>
       <c r="E44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="F44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -992,27 +983,27 @@
         <v>270.2</v>
       </c>
       <c r="C45">
-        <f t="shared" ref="C45:E45" si="2">C44+40*4</f>
+        <f t="shared" ref="C45:E45" si="3">C44+40*4</f>
         <v>262.2</v>
       </c>
       <c r="D45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>259.39999999999998</v>
       </c>
       <c r="E45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>157</v>
       </c>
       <c r="F45">
-        <f t="shared" ref="F45" si="3">F44+40*4</f>
+        <f t="shared" ref="F45" si="4">F44+40*4</f>
         <v>157</v>
       </c>
       <c r="G45">
-        <f t="shared" ref="G45" si="4">G44+40*4</f>
+        <f t="shared" ref="G45" si="5">G44+40*4</f>
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1025,23 +1016,23 @@
         <v>93.642857142857139</v>
       </c>
       <c r="D46">
-        <f t="shared" ref="D46:G46" si="5">D45/2.8</f>
+        <f t="shared" ref="D46:G46" si="6">D45/2.8</f>
         <v>92.642857142857139</v>
       </c>
       <c r="E46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56.071428571428577</v>
       </c>
       <c r="F46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56.071428571428577</v>
       </c>
       <c r="G46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56.071428571428577</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -1050,32 +1041,32 @@
         <v>97</v>
       </c>
       <c r="C47">
-        <f t="shared" ref="C47:G47" si="6">ROUND(C46,0)</f>
+        <f t="shared" ref="C47:G47" si="7">ROUND(C46,0)</f>
         <v>94</v>
       </c>
       <c r="D47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>93</v>
       </c>
       <c r="E47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
       <c r="F47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
       <c r="G47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I48" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -1084,11 +1075,11 @@
         <v>273.2</v>
       </c>
       <c r="C49">
-        <f t="shared" ref="C49:G49" si="7">C45+3</f>
+        <f t="shared" ref="C49:D49" si="8">C45+3</f>
         <v>265.2</v>
       </c>
       <c r="D49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>262.39999999999998</v>
       </c>
       <c r="E49">
@@ -1109,7 +1100,7 @@
         <v>13.346666666666666</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -1118,23 +1109,23 @@
         <v>271.59999999999997</v>
       </c>
       <c r="C50">
-        <f t="shared" ref="C50:G50" si="8">C47*2.8</f>
+        <f t="shared" ref="C50:G50" si="9">C47*2.8</f>
         <v>263.2</v>
       </c>
       <c r="D50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>260.39999999999998</v>
       </c>
       <c r="E50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>156.79999999999998</v>
       </c>
       <c r="F50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>156.79999999999998</v>
       </c>
       <c r="G50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>156.79999999999998</v>
       </c>
       <c r="H50">
@@ -1146,7 +1137,7 @@
         <v>1283.5999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -1155,31 +1146,31 @@
         <v>1.6000000000000227</v>
       </c>
       <c r="C51">
-        <f t="shared" ref="C51:H51" si="9">C49-C50</f>
+        <f t="shared" ref="C51:H51" si="10">C49-C50</f>
         <v>2</v>
       </c>
       <c r="D51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="E51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-156.79999999999998</v>
       </c>
       <c r="F51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-156.79999999999998</v>
       </c>
       <c r="G51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-156.79999999999998</v>
       </c>
       <c r="H51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-464.79999999999995</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D52">
         <f>D51-2.8</f>
         <v>-0.79999999999999982</v>
@@ -1189,32 +1180,32 @@
         <v>-159.6</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>16</v>
       </c>
@@ -1232,9 +1223,9 @@
       <selection activeCell="B25" sqref="B25:G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1680</v>
       </c>
@@ -1254,7 +1245,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1680</v>
       </c>
@@ -1274,7 +1265,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1680</v>
       </c>
@@ -1294,7 +1285,7 @@
         <v>2240</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>4760</v>
       </c>
@@ -1314,7 +1305,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1680</v>
       </c>
@@ -1334,7 +1325,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3360</v>
       </c>
@@ -1354,7 +1345,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1960</v>
       </c>
@@ -1374,7 +1365,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1960</v>
       </c>
@@ -1394,7 +1385,7 @@
         <v>4760</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1400</v>
       </c>
@@ -1414,7 +1405,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2240</v>
       </c>
@@ -1434,7 +1425,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>3080</v>
       </c>
@@ -1454,7 +1445,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>3080</v>
       </c>
@@ -1474,7 +1465,7 @@
         <v>2240</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>3640</v>
       </c>
@@ -1494,7 +1485,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1960</v>
       </c>
@@ -1514,7 +1505,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2520</v>
       </c>
@@ -1534,7 +1525,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1680</v>
       </c>
@@ -1554,7 +1545,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2520</v>
       </c>
@@ -1574,7 +1565,7 @@
         <v>2240</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>3640</v>
       </c>
@@ -1594,7 +1585,7 @@
         <v>4480</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>1960</v>
       </c>
@@ -1614,7 +1605,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>17000</v>
       </c>
@@ -1634,7 +1625,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1642,7 +1633,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +1662,7 @@
         <v>65160</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1700,7 +1691,7 @@
         <v>65.16</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1729,7 +1720,7 @@
         <v>62.16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1758,7 +1749,7 @@
         <v>142.16</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1787,7 +1778,7 @@
         <v>50.771428571428572</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1814,7 +1805,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -1847,7 +1838,7 @@
         <v>856.84000000000015</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1880,7 +1871,7 @@
         <v>845.59999999999991</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -1913,32 +1904,32 @@
         <v>11.240000000000236</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>16</v>
       </c>
@@ -1950,15 +1941,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E52045E-6334-4E6A-B6BC-CE2B6066FCAD}">
-  <dimension ref="A1:K92"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1400</v>
       </c>
@@ -1972,7 +1963,7 @@
         <v>6160</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>280</v>
       </c>
@@ -1986,7 +1977,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>560</v>
       </c>
@@ -2000,7 +1991,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>840</v>
       </c>
@@ -2014,7 +2005,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>280</v>
       </c>
@@ -2028,7 +2019,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1680</v>
       </c>
@@ -2042,7 +2033,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2240</v>
       </c>
@@ -2056,7 +2047,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1120</v>
       </c>
@@ -2070,7 +2061,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2240</v>
       </c>
@@ -2084,7 +2075,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1120</v>
       </c>
@@ -2098,7 +2089,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>840</v>
       </c>
@@ -2112,7 +2103,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9520</v>
       </c>
@@ -2126,7 +2117,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1680</v>
       </c>
@@ -2140,7 +2131,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>8120</v>
       </c>
@@ -2154,7 +2145,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>3360</v>
       </c>
@@ -2168,7 +2159,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1400</v>
       </c>
@@ -2182,7 +2173,7 @@
         <v>6160</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>1400</v>
       </c>
@@ -2196,7 +2187,7 @@
         <v>6160</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>280</v>
       </c>
@@ -2210,7 +2201,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>560</v>
       </c>
@@ -2224,7 +2215,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>840</v>
       </c>
@@ -2238,7 +2229,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>280</v>
       </c>
@@ -2252,7 +2243,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>1680</v>
       </c>
@@ -2266,7 +2257,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>2240</v>
       </c>
@@ -2280,7 +2271,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1120</v>
       </c>
@@ -2294,7 +2285,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>2240</v>
       </c>
@@ -2308,7 +2299,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>1120</v>
       </c>
@@ -2322,7 +2313,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>840</v>
       </c>
@@ -2336,7 +2327,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>9520</v>
       </c>
@@ -2350,7 +2341,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>1680</v>
       </c>
@@ -2364,7 +2355,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>8120</v>
       </c>
@@ -2378,7 +2369,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>3360</v>
       </c>
@@ -2392,7 +2383,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>1400</v>
       </c>
@@ -2406,7 +2397,7 @@
         <v>6160</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>280</v>
       </c>
@@ -2420,7 +2411,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>560</v>
       </c>
@@ -2434,7 +2425,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>840</v>
       </c>
@@ -2448,7 +2439,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>280</v>
       </c>
@@ -2462,7 +2453,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>1680</v>
       </c>
@@ -2476,7 +2467,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>2240</v>
       </c>
@@ -2490,7 +2481,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>1120</v>
       </c>
@@ -2504,7 +2495,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>2240</v>
       </c>
@@ -2518,7 +2509,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>1120</v>
       </c>
@@ -2532,7 +2523,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>840</v>
       </c>
@@ -2546,7 +2537,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>9520</v>
       </c>
@@ -2560,7 +2551,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>1680</v>
       </c>
@@ -2574,7 +2565,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>8120</v>
       </c>
@@ -2588,7 +2579,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>840</v>
       </c>
@@ -2602,7 +2593,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>9520</v>
       </c>
@@ -2616,7 +2607,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>17000</v>
       </c>
@@ -2630,7 +2621,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -2638,7 +2629,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -2675,7 +2666,7 @@
         <v>7.4126666666666674</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -2712,7 +2703,7 @@
         <v>7.4126666666666664E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -2749,7 +2740,7 @@
         <v>7.1126666666666664E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -2786,7 +2777,7 @@
         <v>2.6312666666666665E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -2823,7 +2814,7 @@
         <v>9.3973809523809522E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -2852,7 +2843,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -2861,7 +2852,7 @@
         <v>324.24</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:G57" si="12">C53+3</f>
+        <f t="shared" ref="C57:E57" si="12">C53+3</f>
         <v>298.88</v>
       </c>
       <c r="D57">
@@ -2887,7 +2878,7 @@
         <v>20.212666666666667</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -2920,7 +2911,7 @@
         <v>1584.8000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -2953,7 +2944,7 @@
         <v>-372.04000000000019</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C60">
         <f>C59-2.8</f>
         <v>-0.7199999999999589</v>
@@ -2967,34 +2958,6 @@
         <v>-0.72000000000001574</v>
       </c>
     </row>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3004,13 +2967,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143618EE-F9B7-44E1-A7E5-9C4E4B882B94}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:E41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>560</v>
       </c>
@@ -3024,7 +2987,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1120</v>
       </c>
@@ -3038,7 +3001,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1960</v>
       </c>
@@ -3052,7 +3015,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2800</v>
       </c>
@@ -3066,7 +3029,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1400</v>
       </c>
@@ -3080,7 +3043,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>560</v>
       </c>
@@ -3094,7 +3057,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>840</v>
       </c>
@@ -3108,7 +3071,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1680</v>
       </c>
@@ -3122,7 +3085,7 @@
         <v>4480</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>560</v>
       </c>
@@ -3136,7 +3099,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>280</v>
       </c>
@@ -3150,7 +3113,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>840</v>
       </c>
@@ -3164,7 +3127,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>7280</v>
       </c>
@@ -3178,7 +3141,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>3640</v>
       </c>
@@ -3192,7 +3155,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>3640</v>
       </c>
@@ -3206,7 +3169,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>5040</v>
       </c>
@@ -3220,7 +3183,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1960</v>
       </c>
@@ -3234,7 +3197,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>560</v>
       </c>
@@ -3248,7 +3211,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1120</v>
       </c>
@@ -3262,7 +3225,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>1960</v>
       </c>
@@ -3276,7 +3239,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2800</v>
       </c>
@@ -3290,7 +3253,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>1400</v>
       </c>
@@ -3304,7 +3267,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>560</v>
       </c>
@@ -3318,7 +3281,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>840</v>
       </c>
@@ -3332,7 +3295,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1680</v>
       </c>
@@ -3346,7 +3309,7 @@
         <v>4480</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>560</v>
       </c>
@@ -3360,7 +3323,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>280</v>
       </c>
@@ -3374,7 +3337,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>840</v>
       </c>
@@ -3388,7 +3351,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>7280</v>
       </c>
@@ -3402,7 +3365,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>3640</v>
       </c>
@@ -3416,7 +3379,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>3640</v>
       </c>
@@ -3430,7 +3393,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>5040</v>
       </c>
@@ -3444,7 +3407,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>17000</v>
       </c>
@@ -3458,7 +3421,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -3466,7 +3429,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -3487,7 +3450,7 @@
         <v>64880</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -3508,7 +3471,7 @@
         <v>64.88</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -3529,152 +3492,152 @@
         <v>61.879999999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>2</v>
       </c>
       <c r="B41">
-        <f>B40+32*4</f>
-        <v>209.36</v>
+        <f>B40+32*2.5</f>
+        <v>161.36000000000001</v>
       </c>
       <c r="C41">
-        <f t="shared" ref="C41:E41" si="3">C40+32*4</f>
-        <v>197.72</v>
+        <f t="shared" ref="C41:E41" si="3">C40+32*2.5</f>
+        <v>149.72</v>
       </c>
       <c r="D41">
         <f t="shared" si="3"/>
-        <v>213.95999999999998</v>
+        <v>165.95999999999998</v>
       </c>
       <c r="E41">
         <f t="shared" si="3"/>
-        <v>189.88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>141.88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
       <c r="B42">
         <f>B41/2.8</f>
-        <v>74.771428571428586</v>
+        <v>57.628571428571441</v>
       </c>
       <c r="C42">
         <f>C41/2.8</f>
-        <v>70.614285714285714</v>
+        <v>53.471428571428575</v>
       </c>
       <c r="D42">
         <f t="shared" ref="D42:E42" si="4">D41/2.8</f>
-        <v>76.414285714285711</v>
+        <v>59.271428571428565</v>
       </c>
       <c r="E42">
         <f t="shared" si="4"/>
-        <v>67.814285714285717</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>50.671428571428571</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
       <c r="B43">
         <f>ROUND(B42,0)</f>
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C43">
         <f t="shared" ref="C43:E43" si="5">ROUND(C42,0)</f>
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D43">
         <f t="shared" si="5"/>
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E43">
         <f t="shared" si="5"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
       <c r="B45">
         <f>B41+3</f>
-        <v>212.36</v>
+        <v>164.36</v>
       </c>
       <c r="C45">
         <f t="shared" ref="C45:E45" si="6">C41+3</f>
-        <v>200.72</v>
+        <v>152.72</v>
       </c>
       <c r="D45">
         <f t="shared" si="6"/>
-        <v>216.95999999999998</v>
+        <v>168.95999999999998</v>
       </c>
       <c r="E45">
         <f t="shared" si="6"/>
-        <v>192.88</v>
+        <v>144.88</v>
       </c>
       <c r="H45">
         <f>SUM(B45:G45)</f>
-        <v>822.92</v>
+        <v>630.92000000000007</v>
       </c>
       <c r="I45">
         <f>H45/60</f>
-        <v>13.715333333333332</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10.515333333333334</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
       <c r="B46">
         <f>B43*2.8</f>
-        <v>210</v>
+        <v>162.39999999999998</v>
       </c>
       <c r="C46">
         <f t="shared" ref="C46:E46" si="7">C43*2.8</f>
-        <v>198.79999999999998</v>
+        <v>148.39999999999998</v>
       </c>
       <c r="D46">
         <f t="shared" si="7"/>
-        <v>212.79999999999998</v>
+        <v>165.2</v>
       </c>
       <c r="E46">
         <f t="shared" si="7"/>
-        <v>190.39999999999998</v>
+        <v>142.79999999999998</v>
       </c>
       <c r="H46">
         <f>SUM(B46:G46)</f>
-        <v>811.99999999999989</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+        <v>618.79999999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>15</v>
       </c>
       <c r="B47">
         <f>B45-B46</f>
-        <v>2.3600000000000136</v>
+        <v>1.9600000000000364</v>
       </c>
       <c r="C47">
         <f t="shared" ref="C47:H47" si="8">C45-C46</f>
-        <v>1.9200000000000159</v>
+        <v>4.3200000000000216</v>
       </c>
       <c r="D47">
         <f t="shared" si="8"/>
-        <v>4.1599999999999966</v>
+        <v>3.7599999999999909</v>
       </c>
       <c r="E47">
         <f t="shared" si="8"/>
-        <v>2.4800000000000182</v>
+        <v>2.0800000000000125</v>
       </c>
       <c r="H47">
         <f t="shared" si="8"/>
-        <v>10.920000000000073</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.120000000000118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48">
         <f>B47-2.8</f>
-        <v>-0.43999999999998618</v>
+        <v>-0.83999999999996344</v>
       </c>
     </row>
   </sheetData>
@@ -3690,9 +3653,9 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>560</v>
       </c>
@@ -3706,7 +3669,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1120</v>
       </c>
@@ -3720,7 +3683,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1960</v>
       </c>
@@ -3734,7 +3697,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2800</v>
       </c>
@@ -3748,7 +3711,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1400</v>
       </c>
@@ -3762,7 +3725,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>560</v>
       </c>
@@ -3776,7 +3739,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>840</v>
       </c>
@@ -3790,7 +3753,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1680</v>
       </c>
@@ -3804,7 +3767,7 @@
         <v>4480</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>560</v>
       </c>
@@ -3818,7 +3781,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>280</v>
       </c>
@@ -3832,7 +3795,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>840</v>
       </c>
@@ -3846,7 +3809,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>7280</v>
       </c>
@@ -3860,7 +3823,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>3640</v>
       </c>
@@ -3874,7 +3837,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>3640</v>
       </c>
@@ -3888,7 +3851,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>5040</v>
       </c>
@@ -3902,7 +3865,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>17000</v>
       </c>
@@ -3916,7 +3879,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -3924,7 +3887,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -3945,7 +3908,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -3966,7 +3929,7 @@
         <v>40.520000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -3987,7 +3950,7 @@
         <v>37.520000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -4008,7 +3971,7 @@
         <v>117.52000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -4029,7 +3992,7 @@
         <v>41.971428571428575</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -4049,7 +4012,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -4074,7 +4037,7 @@
         <v>505.76</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -4099,7 +4062,7 @@
         <v>495.6</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>

</xml_diff>